<commit_message>
Añadidas nuevas configuraciones de reflectancia mediadas con espectrómetro (AB F2)
</commit_message>
<xml_diff>
--- a/DB_folder/Configuracion_Reflectancias_DB.xlsx
+++ b/DB_folder/Configuracion_Reflectancias_DB.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Estándar" sheetId="1" r:id="rId1"/>
     <sheet name="Vol 1 Algerri-B" sheetId="2" r:id="rId2"/>
     <sheet name="Vol 2 Algerri-B" sheetId="3" r:id="rId3"/>
+    <sheet name="AB F2 C1" sheetId="4" r:id="rId4"/>
+    <sheet name="AB F2 C2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="9">
   <si>
     <t>Master</t>
   </si>
@@ -49,7 +51,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,16 +59,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -74,12 +88,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,9 +424,9 @@
       <selection activeCell="C18" sqref="A1:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,7 +437,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -411,7 +445,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -419,7 +453,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -430,7 +464,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -438,7 +472,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -446,7 +480,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -457,7 +491,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -465,7 +499,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -473,7 +507,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -484,7 +518,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -492,7 +526,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -500,7 +534,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -511,7 +545,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>2</v>
       </c>
@@ -519,7 +553,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -527,7 +561,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -538,7 +572,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -546,7 +580,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -567,9 +601,9 @@
       <selection activeCell="C18" sqref="A1:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -580,7 +614,7 @@
         <v>0.90515213999999999</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -588,7 +622,7 @@
         <v>5.5214909999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -596,7 +630,7 @@
         <v>0.13521490999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -607,7 +641,7 @@
         <v>0.45021334000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -615,7 +649,7 @@
         <v>2.6949312999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -623,7 +657,7 @@
         <v>0.106949313</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -634,7 +668,7 @@
         <v>0.62777810000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -642,7 +676,7 @@
         <v>3.8630289999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -650,7 +684,7 @@
         <v>0.11863029</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -661,7 +695,7 @@
         <v>0.75442629999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -669,7 +703,7 @@
         <v>4.3311179999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -677,7 +711,7 @@
         <v>0.12331118000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -688,7 +722,7 @@
         <v>0.7750011</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>2</v>
       </c>
@@ -696,7 +730,7 @@
         <v>4.4679402999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -704,7 +738,7 @@
         <v>0.12467940299999999</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -715,7 +749,7 @@
         <v>0.74113667000000005</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -723,7 +757,7 @@
         <v>4.3302737000000001E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -740,13 +774,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -757,7 +791,7 @@
         <v>0.86227750000000003</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -765,7 +799,7 @@
         <v>5.1412694000000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -773,7 +807,7 @@
         <v>0.131412694</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -784,7 +818,7 @@
         <v>0.58787460000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -792,7 +826,7 @@
         <v>3.6282920000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -800,7 +834,7 @@
         <v>0.11628292</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -811,7 +845,7 @@
         <v>0.65672680000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -819,7 +853,7 @@
         <v>4.0654679999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -827,7 +861,7 @@
         <v>0.12065468</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -838,7 +872,7 @@
         <v>0.75442629999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -846,7 +880,7 @@
         <v>4.3311179999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -854,7 +888,7 @@
         <v>0.12331118000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -865,7 +899,7 @@
         <v>0.7750011</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>2</v>
       </c>
@@ -873,7 +907,7 @@
         <v>4.4679402999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -881,7 +915,7 @@
         <v>0.12467940299999999</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -892,7 +926,7 @@
         <v>0.76641550000000003</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -900,12 +934,378 @@
         <v>4.4257589999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>3</v>
       </c>
       <c r="C18">
         <v>0.12425759</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>0.97478600000000004</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>5.7932664000000002E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>5.7932664000000002E-2</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0.98143332999999999</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>5.9950656999999997E-2</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>5.9950656999999997E-2</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0.97732686999999996</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>5.6798395000000002E-2</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>5.6798395000000002E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0.97616583000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>5.6885353999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>5.6885353999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0.97760623999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>5.9006485999999997E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>5.9006485999999997E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0.97913724000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>6.0097563999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>6.0097563999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>0.97502690000000003</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>5.9658673000000002E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>5.9658673000000002E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0.97899216</v>
+      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>5.6465614999999997E-2</v>
+      </c>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>5.6465614999999997E-2</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0.97554129999999994</v>
+      </c>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>5.6221712E-2</v>
+      </c>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>5.6221712E-2</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0.97616583000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>5.6885353999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>5.6885353999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0.97757740000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>5.9187820000000002E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>5.9187820000000002E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Añadido programa para uso de un solo radioespectrómetro
</commit_message>
<xml_diff>
--- a/DB_folder/Configuracion_Reflectancias_DB.xlsx
+++ b/DB_folder/Configuracion_Reflectancias_DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Estándar" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,15 @@
     <sheet name="Vol 2 Algerri-B" sheetId="3" r:id="rId3"/>
     <sheet name="AB F2 C1" sheetId="4" r:id="rId4"/>
     <sheet name="AB F2 C2" sheetId="5" r:id="rId5"/>
+    <sheet name="Verif Payloads C1" sheetId="6" r:id="rId6"/>
+    <sheet name="Verif Payloads C2" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="9">
   <si>
     <t>Master</t>
   </si>
@@ -424,9 +426,9 @@
       <selection activeCell="C18" sqref="A1:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,7 +439,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -445,7 +447,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -453,7 +455,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -464,7 +466,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -472,7 +474,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -480,7 +482,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -491,7 +493,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -499,7 +501,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -507,7 +509,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -518,7 +520,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -526,7 +528,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -534,7 +536,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -545,7 +547,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>2</v>
       </c>
@@ -553,7 +555,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -561,7 +563,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -572,7 +574,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -580,7 +582,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -601,9 +603,9 @@
       <selection activeCell="C18" sqref="A1:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -614,7 +616,7 @@
         <v>0.90515213999999999</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -622,7 +624,7 @@
         <v>5.5214909999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -630,7 +632,7 @@
         <v>0.13521490999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -641,7 +643,7 @@
         <v>0.45021334000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -649,7 +651,7 @@
         <v>2.6949312999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -657,7 +659,7 @@
         <v>0.106949313</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -668,7 +670,7 @@
         <v>0.62777810000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -676,7 +678,7 @@
         <v>3.8630289999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -684,7 +686,7 @@
         <v>0.11863029</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -695,7 +697,7 @@
         <v>0.75442629999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -703,7 +705,7 @@
         <v>4.3311179999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -711,7 +713,7 @@
         <v>0.12331118000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -722,7 +724,7 @@
         <v>0.7750011</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>2</v>
       </c>
@@ -730,7 +732,7 @@
         <v>4.4679402999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -738,7 +740,7 @@
         <v>0.12467940299999999</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -749,7 +751,7 @@
         <v>0.74113667000000005</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -757,7 +759,7 @@
         <v>4.3302737000000001E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -778,9 +780,9 @@
       <selection sqref="A1:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -791,7 +793,7 @@
         <v>0.86227750000000003</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -799,7 +801,7 @@
         <v>5.1412694000000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -807,7 +809,7 @@
         <v>0.131412694</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -818,7 +820,7 @@
         <v>0.58787460000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -826,7 +828,7 @@
         <v>3.6282920000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -834,7 +836,7 @@
         <v>0.11628292</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -845,7 +847,7 @@
         <v>0.65672680000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -853,7 +855,7 @@
         <v>4.0654679999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -861,7 +863,7 @@
         <v>0.12065468</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -872,7 +874,7 @@
         <v>0.75442629999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -880,7 +882,7 @@
         <v>4.3311179999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -888,7 +890,7 @@
         <v>0.12331118000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -899,7 +901,7 @@
         <v>0.7750011</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>2</v>
       </c>
@@ -907,7 +909,7 @@
         <v>4.4679402999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -915,7 +917,7 @@
         <v>0.12467940299999999</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -926,7 +928,7 @@
         <v>0.76641550000000003</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -934,7 +936,7 @@
         <v>4.4257589999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -951,13 +953,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="A1:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -968,7 +970,7 @@
         <v>0.97478600000000004</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -976,7 +978,7 @@
         <v>5.7932664000000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -985,7 +987,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -997,7 +999,7 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -1006,7 +1008,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1015,7 +1017,7 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1027,7 +1029,7 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -1036,7 +1038,7 @@
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -1044,7 +1046,7 @@
         <v>5.6798395000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1055,7 +1057,7 @@
         <v>0.97616583000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -1063,7 +1065,7 @@
         <v>5.6885353999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -1071,7 +1073,7 @@
         <v>5.6885353999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1082,7 +1084,7 @@
         <v>0.97760623999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>2</v>
       </c>
@@ -1090,7 +1092,7 @@
         <v>5.9006485999999997E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -1098,7 +1100,7 @@
         <v>5.9006485999999997E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1109,7 +1111,7 @@
         <v>0.97913724000000002</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -1117,7 +1119,7 @@
         <v>6.0097563999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -1135,12 +1137,12 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection sqref="A1:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1151,7 +1153,7 @@
         <v>0.97502690000000003</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -1159,7 +1161,7 @@
         <v>5.9658673000000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -1167,7 +1169,7 @@
         <v>5.9658673000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1179,7 +1181,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -1188,7 +1190,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1197,7 +1199,7 @@
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1209,7 +1211,7 @@
       </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -1218,7 +1220,7 @@
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -1227,7 +1229,7 @@
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1238,7 +1240,7 @@
         <v>0.97616583000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -1246,7 +1248,7 @@
         <v>5.6885353999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -1254,7 +1256,7 @@
         <v>5.6885353999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1265,7 +1267,7 @@
         <v>0.97757740000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>2</v>
       </c>
@@ -1273,7 +1275,7 @@
         <v>5.9187820000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -1281,7 +1283,7 @@
         <v>5.9187820000000002E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1292,7 +1294,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -1300,7 +1302,361 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>0.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>5.9658673000000002E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>5.6465614999999997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>5.6221712E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>5.6885353999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>5.9187820000000002E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>0.06</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>5.9658673000000002E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>5.8000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>5.6465614999999997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>5.8000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>5.6221712E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>5.7000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>5.6885353999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>5.8000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>5.9187820000000002E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>5.8999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Añadida config reflectancias de M2 Drone FB
</commit_message>
<xml_diff>
--- a/DB_folder/Configuracion_Reflectancias_DB.xlsx
+++ b/DB_folder/Configuracion_Reflectancias_DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="1176" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Estándar" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="AB F2 C2" sheetId="5" r:id="rId5"/>
     <sheet name="Verif Payloads C1" sheetId="6" r:id="rId6"/>
     <sheet name="Verif Payloads C2" sheetId="7" r:id="rId7"/>
+    <sheet name="M2 Drone FB" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="9">
   <si>
     <t>Master</t>
   </si>
@@ -1496,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="A1:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1667,4 +1668,181 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>5.9658673000000002E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>4.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>5.6465614999999997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>4.9000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>5.6221712E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>5.6885353999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>5.9187820000000002E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>